<commit_message>
laksdjalksdj update feriswhel excel
</commit_message>
<xml_diff>
--- a/ferrisWheel/2dparts_schematic_materials-fer.xlsx
+++ b/ferrisWheel/2dparts_schematic_materials-fer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\ferrisWheel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534CBCA9-A68E-4F93-940E-71527BD6BE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBBF7D2-1BEE-43AE-AEB7-2C138D9607B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>motor</t>
   </si>
@@ -120,13 +120,34 @@
   </si>
   <si>
     <t>2d parts</t>
+  </si>
+  <si>
+    <t>Overview motor to ferris wheel</t>
+  </si>
+  <si>
+    <t>Part L</t>
+  </si>
+  <si>
+    <t>Part M</t>
+  </si>
+  <si>
+    <t>Part N</t>
+  </si>
+  <si>
+    <t>Big wheel</t>
+  </si>
+  <si>
+    <t>string interface</t>
+  </si>
+  <si>
+    <t>Stand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +171,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -167,17 +216,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,6 +719,189 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758B7254-FF67-4F90-B348-A575196AD8C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="10386060"/>
+          <a:ext cx="2613660" cy="2590800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F17E77A-FBE4-4075-B4B5-CC3FD991C3A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2766060" y="11203288"/>
+          <a:ext cx="762000" cy="836312"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Isosceles Triangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE21716-9321-02A6-793A-7F6A7E6B570A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2255520" y="11666220"/>
+          <a:ext cx="1828800" cy="1615440"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -923,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046D2DF6-7029-4E01-AB00-EF8208A806E9}">
   <dimension ref="A2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,40 +1299,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
-  <dimension ref="B2:N46"/>
+  <dimension ref="B2:R61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:18" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="N11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
         <v>25</v>
       </c>
@@ -1086,7 +1376,25 @@
         <v>19</v>
       </c>
     </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N11:R11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1094,18 +1402,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB8265-3C8E-4609-81CC-B5279E8DC9E7}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>